<commit_message>
upadate *.xlsx, and *.csv.
</commit_message>
<xml_diff>
--- a/data/BT_books.xlsx
+++ b/data/BT_books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.91.11\Share\node_Book\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\book.rp.lfx.sony.co.jp\Share\node_Book\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54087D1B-54F4-411C-B610-8468B9984BD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{714DAAA1-1A1E-48BA-8F97-A699F7A0F3E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25365" windowHeight="12510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25365" windowHeight="12510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="備品" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="669">
   <si>
     <t>品名・種類</t>
   </si>
@@ -2281,7 +2281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2477,6 +2477,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2875,7 +2876,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2892,7 +2893,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="74"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2907,7 +2908,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="74"/>
+      <c r="A5" s="75"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -2922,7 +2923,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="74"/>
+      <c r="A6" s="75"/>
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
@@ -2937,7 +2938,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="74"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
@@ -2952,7 +2953,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="74"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
@@ -2967,7 +2968,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="74" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2987,7 +2988,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="74"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
@@ -3002,7 +3003,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="74"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
@@ -3017,7 +3018,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="74"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
@@ -3032,7 +3033,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="74"/>
+      <c r="A13" s="75"/>
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
@@ -3047,7 +3048,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="74"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
@@ -3062,7 +3063,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="74"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
@@ -3080,7 +3081,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="74"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
@@ -3096,7 +3097,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="74"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
@@ -3114,7 +3115,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="74" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3131,7 +3132,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="74"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="4" t="s">
         <v>50</v>
       </c>
@@ -3163,7 +3164,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="74" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -3183,7 +3184,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A22" s="74"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
@@ -3219,7 +3220,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="74" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -3239,7 +3240,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="74"/>
+      <c r="A25" s="75"/>
       <c r="B25" s="4" t="s">
         <v>69</v>
       </c>
@@ -3257,7 +3258,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A26" s="74"/>
+      <c r="A26" s="75"/>
       <c r="B26" s="4" t="s">
         <v>72</v>
       </c>
@@ -3275,7 +3276,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A27" s="74"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="4" t="s">
         <v>74</v>
       </c>
@@ -3293,7 +3294,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A28" s="74"/>
+      <c r="A28" s="75"/>
       <c r="B28" s="4" t="s">
         <v>76</v>
       </c>
@@ -3311,7 +3312,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A29" s="74"/>
+      <c r="A29" s="75"/>
       <c r="B29" s="4" t="s">
         <v>78</v>
       </c>
@@ -3329,7 +3330,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="74" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -3346,7 +3347,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A31" s="74"/>
+      <c r="A31" s="75"/>
       <c r="B31" s="4" t="s">
         <v>90</v>
       </c>
@@ -3414,7 +3415,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75">
-      <c r="A35" s="73" t="s">
+      <c r="A35" s="74" t="s">
         <v>106</v>
       </c>
       <c r="B35" s="20" t="s">
@@ -3432,7 +3433,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75">
-      <c r="A36" s="74"/>
+      <c r="A36" s="75"/>
       <c r="B36" s="20" t="s">
         <v>109</v>
       </c>
@@ -3448,7 +3449,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75">
-      <c r="A37" s="74"/>
+      <c r="A37" s="75"/>
       <c r="B37" s="20" t="s">
         <v>113</v>
       </c>
@@ -3466,7 +3467,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75">
-      <c r="A38" s="74"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="20" t="s">
         <v>122</v>
       </c>
@@ -3484,7 +3485,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75">
-      <c r="A39" s="74"/>
+      <c r="A39" s="75"/>
       <c r="B39" s="20" t="s">
         <v>126</v>
       </c>
@@ -3500,7 +3501,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75">
-      <c r="A40" s="74"/>
+      <c r="A40" s="75"/>
       <c r="B40" s="20" t="s">
         <v>127</v>
       </c>
@@ -3516,7 +3517,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75">
-      <c r="A41" s="74"/>
+      <c r="A41" s="75"/>
       <c r="B41" s="20" t="s">
         <v>128</v>
       </c>
@@ -3532,7 +3533,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="12.75">
-      <c r="A42" s="74"/>
+      <c r="A42" s="75"/>
       <c r="B42" s="20" t="s">
         <v>130</v>
       </c>
@@ -3600,7 +3601,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75">
-      <c r="A46" s="73" t="s">
+      <c r="A46" s="74" t="s">
         <v>139</v>
       </c>
       <c r="B46" s="20"/>
@@ -3614,7 +3615,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" ht="12.75">
-      <c r="A47" s="74"/>
+      <c r="A47" s="75"/>
       <c r="B47" s="20"/>
       <c r="C47" s="21">
         <v>5</v>
@@ -3628,7 +3629,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="74" t="s">
         <v>141</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -3646,7 +3647,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75">
-      <c r="A49" s="74"/>
+      <c r="A49" s="75"/>
       <c r="B49" s="20" t="s">
         <v>144</v>
       </c>
@@ -3662,7 +3663,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75">
-      <c r="A50" s="74"/>
+      <c r="A50" s="75"/>
       <c r="B50" s="20" t="s">
         <v>146</v>
       </c>
@@ -3678,7 +3679,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75">
-      <c r="A51" s="74"/>
+      <c r="A51" s="75"/>
       <c r="B51" s="20" t="s">
         <v>147</v>
       </c>
@@ -3696,7 +3697,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75">
-      <c r="A52" s="74"/>
+      <c r="A52" s="75"/>
       <c r="B52" s="20" t="s">
         <v>150</v>
       </c>
@@ -3714,7 +3715,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75">
-      <c r="A53" s="74"/>
+      <c r="A53" s="75"/>
       <c r="B53" s="20" t="s">
         <v>154</v>
       </c>
@@ -3732,7 +3733,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75">
-      <c r="A54" s="74"/>
+      <c r="A54" s="75"/>
       <c r="B54" s="20" t="s">
         <v>156</v>
       </c>
@@ -3748,7 +3749,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75">
-      <c r="A55" s="74"/>
+      <c r="A55" s="75"/>
       <c r="B55" s="20" t="s">
         <v>160</v>
       </c>
@@ -3784,7 +3785,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75">
-      <c r="A57" s="73" t="s">
+      <c r="A57" s="74" t="s">
         <v>171</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -3804,7 +3805,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.75">
-      <c r="A58" s="74"/>
+      <c r="A58" s="75"/>
       <c r="B58" s="4" t="s">
         <v>175</v>
       </c>
@@ -3822,7 +3823,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75">
-      <c r="A59" s="74"/>
+      <c r="A59" s="75"/>
       <c r="B59" s="4" t="s">
         <v>178</v>
       </c>
@@ -3840,7 +3841,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75">
-      <c r="A60" s="74"/>
+      <c r="A60" s="75"/>
       <c r="B60" s="4" t="s">
         <v>181</v>
       </c>
@@ -3856,7 +3857,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="12.75">
-      <c r="A61" s="74"/>
+      <c r="A61" s="75"/>
       <c r="B61" s="4" t="s">
         <v>182</v>
       </c>
@@ -3872,7 +3873,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75">
-      <c r="A62" s="74"/>
+      <c r="A62" s="75"/>
       <c r="B62" s="4" t="s">
         <v>185</v>
       </c>
@@ -3888,7 +3889,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75">
-      <c r="A63" s="74"/>
+      <c r="A63" s="75"/>
       <c r="B63" s="4" t="s">
         <v>186</v>
       </c>
@@ -3906,7 +3907,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75">
-      <c r="A64" s="73" t="s">
+      <c r="A64" s="74" t="s">
         <v>188</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -3923,7 +3924,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="12.75">
-      <c r="A65" s="74"/>
+      <c r="A65" s="75"/>
       <c r="B65" s="4" t="s">
         <v>191</v>
       </c>
@@ -3938,7 +3939,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75">
-      <c r="A66" s="74"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="4" t="s">
         <v>193</v>
       </c>
@@ -3991,7 +3992,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="12.75">
-      <c r="A69" s="73" t="s">
+      <c r="A69" s="74" t="s">
         <v>201</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -4008,7 +4009,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="12.75">
-      <c r="A70" s="74"/>
+      <c r="A70" s="75"/>
       <c r="B70" s="4" t="s">
         <v>205</v>
       </c>
@@ -4026,7 +4027,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="12.75">
-      <c r="A71" s="74"/>
+      <c r="A71" s="75"/>
       <c r="B71" s="4" t="s">
         <v>209</v>
       </c>
@@ -4044,7 +4045,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="12.75">
-      <c r="A72" s="73" t="s">
+      <c r="A72" s="74" t="s">
         <v>212</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -4064,7 +4065,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="12.75">
-      <c r="A73" s="74"/>
+      <c r="A73" s="75"/>
       <c r="B73" s="4" t="s">
         <v>218</v>
       </c>
@@ -4082,7 +4083,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="12.75">
-      <c r="A74" s="74"/>
+      <c r="A74" s="75"/>
       <c r="B74" s="4" t="s">
         <v>220</v>
       </c>
@@ -4100,7 +4101,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="12.75">
-      <c r="A75" s="74"/>
+      <c r="A75" s="75"/>
       <c r="B75" s="4" t="s">
         <v>224</v>
       </c>
@@ -4155,7 +4156,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="12.75">
-      <c r="A78" s="73" t="s">
+      <c r="A78" s="74" t="s">
         <v>149</v>
       </c>
       <c r="B78" s="4" t="s">
@@ -4172,7 +4173,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="12.75">
-      <c r="A79" s="74"/>
+      <c r="A79" s="75"/>
       <c r="B79" s="4" t="s">
         <v>242</v>
       </c>
@@ -10950,6 +10951,11 @@
   </sheetData>
   <autoFilter ref="F1:F1043" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="14">
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A3:A8"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A78:A79"/>
@@ -10959,11 +10965,6 @@
     <mergeCell ref="A69:A71"/>
     <mergeCell ref="A57:A63"/>
     <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <dataValidations count="2">
@@ -15303,16 +15304,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098418B-62F2-4EAA-91E1-9A743328C502}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="8" width="14.42578125" style="62"/>
-    <col min="9" max="9" width="49" style="62" customWidth="1"/>
+    <col min="9" max="9" width="68.85546875" style="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37" style="62" customWidth="1"/>
     <col min="11" max="11" width="17" style="62" customWidth="1"/>
     <col min="12" max="12" width="15.140625" style="62" customWidth="1"/>
@@ -15443,26 +15444,26 @@
       <c r="Q3" s="68"/>
       <c r="R3" s="69"/>
     </row>
-    <row r="4" spans="1:18" ht="24.75">
+    <row r="4" spans="1:18" s="73" customFormat="1" ht="24">
       <c r="A4" s="47" t="b">
         <v>0</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
-      <c r="I4" s="70" t="s">
-        <v>665</v>
+      <c r="I4" s="64" t="s">
+        <v>662</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="K4" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="71" t="s">
-        <v>666</v>
-      </c>
-      <c r="M4" s="72" t="s">
-        <v>55</v>
+      <c r="L4" s="67" t="s">
+        <v>664</v>
+      </c>
+      <c r="M4" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="N4" s="68" t="s">
         <v>14</v>
@@ -15476,24 +15477,26 @@
       <c r="Q4" s="68"/>
       <c r="R4" s="69"/>
     </row>
-    <row r="5" spans="1:18" ht="24.75">
+    <row r="5" spans="1:18" s="73" customFormat="1" ht="24">
       <c r="A5" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="70" t="s">
-        <v>665</v>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="I5" s="64" t="s">
+        <v>662</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="K5" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="71" t="s">
-        <v>666</v>
-      </c>
-      <c r="M5" s="72" t="s">
-        <v>55</v>
+      <c r="L5" s="67" t="s">
+        <v>664</v>
+      </c>
+      <c r="M5" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="N5" s="68" t="s">
         <v>14</v>
@@ -15507,24 +15510,26 @@
       <c r="Q5" s="68"/>
       <c r="R5" s="69"/>
     </row>
-    <row r="6" spans="1:18" ht="24.75">
+    <row r="6" spans="1:18" s="73" customFormat="1" ht="24">
       <c r="A6" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="70" t="s">
-        <v>667</v>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="I6" s="64" t="s">
+        <v>662</v>
       </c>
       <c r="J6" s="65" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="K6" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="71" t="s">
-        <v>668</v>
-      </c>
-      <c r="M6" s="72" t="s">
-        <v>65</v>
+      <c r="L6" s="67" t="s">
+        <v>664</v>
+      </c>
+      <c r="M6" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="N6" s="68" t="s">
         <v>14</v>
@@ -15538,24 +15543,26 @@
       <c r="Q6" s="68"/>
       <c r="R6" s="69"/>
     </row>
-    <row r="7" spans="1:18" ht="24.75">
+    <row r="7" spans="1:18" s="73" customFormat="1" ht="24">
       <c r="A7" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="70" t="s">
-        <v>667</v>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="I7" s="64" t="s">
+        <v>662</v>
       </c>
       <c r="J7" s="65" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="K7" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="71" t="s">
-        <v>668</v>
-      </c>
-      <c r="M7" s="72" t="s">
-        <v>65</v>
+      <c r="L7" s="67" t="s">
+        <v>664</v>
+      </c>
+      <c r="M7" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="N7" s="68" t="s">
         <v>14</v>
@@ -15568,17 +15575,207 @@
       </c>
       <c r="Q7" s="68"/>
       <c r="R7" s="69"/>
+    </row>
+    <row r="8" spans="1:18" ht="24.75">
+      <c r="A8" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="I8" s="70" t="s">
+        <v>665</v>
+      </c>
+      <c r="J8" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="71" t="s">
+        <v>666</v>
+      </c>
+      <c r="M8" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="69"/>
+    </row>
+    <row r="9" spans="1:18" ht="24.75">
+      <c r="A9" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="70" t="s">
+        <v>665</v>
+      </c>
+      <c r="J9" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="71" t="s">
+        <v>666</v>
+      </c>
+      <c r="M9" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="69"/>
+    </row>
+    <row r="10" spans="1:18" s="73" customFormat="1" ht="24.75">
+      <c r="A10" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="I10" s="70" t="s">
+        <v>665</v>
+      </c>
+      <c r="J10" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="71" t="s">
+        <v>666</v>
+      </c>
+      <c r="M10" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+    </row>
+    <row r="11" spans="1:18" s="73" customFormat="1" ht="24.75">
+      <c r="A11" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="70" t="s">
+        <v>665</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="71" t="s">
+        <v>666</v>
+      </c>
+      <c r="M11" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="69"/>
+    </row>
+    <row r="12" spans="1:18" ht="24.75">
+      <c r="A12" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="70" t="s">
+        <v>667</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="71" t="s">
+        <v>668</v>
+      </c>
+      <c r="M12" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="69"/>
+    </row>
+    <row r="13" spans="1:18" ht="24.75">
+      <c r="A13" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="70" t="s">
+        <v>667</v>
+      </c>
+      <c r="J13" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="71" t="s">
+        <v>668</v>
+      </c>
+      <c r="M13" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="O2:O7" xr:uid="{E4221C7C-A04A-4151-AD8F-2EE81730CE77}">
+    <dataValidation type="list" allowBlank="1" sqref="O2:O13" xr:uid="{E4221C7C-A04A-4151-AD8F-2EE81730CE77}">
       <formula1>"NEW!,設計・ソフトウェア・DIY,UX・インターフェイス,アイデェア・イノベーション・ビジネスモデル,その他"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="N2:N7" xr:uid="{B41DFE80-A98D-4135-8CD4-2CE325DDC2AC}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N13" xr:uid="{B41DFE80-A98D-4135-8CD4-2CE325DDC2AC}">
       <formula1>"日本語,ENGLISH,その他"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="P2:P7" xr:uid="{554C5BB3-7CB5-4D54-B7AB-C7E6B8AB3E22}">
+    <dataValidation type="list" allowBlank="1" sqref="P2:P13" xr:uid="{554C5BB3-7CB5-4D54-B7AB-C7E6B8AB3E22}">
       <formula1>"単行本,大型本,雑誌,ムック,カタログ,その他"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15591,7 +15788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D7D2A9-31BB-43C6-8C41-A97287F2B06A}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>